<commit_message>
actualización 25 de agosto
</commit_message>
<xml_diff>
--- a/Series/gráficos/graficos.xlsx
+++ b/Series/gráficos/graficos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Github\Camaras\Series\gráficos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E59E8CE-9495-45C4-8D02-1CC9679477C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0ED71A8-4450-4107-9E0E-4064356696F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E6FB40A0-89D6-4DE1-A7CC-889DE5CE92C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6FB40A0-89D6-4DE1-A7CC-889DE5CE92C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>crecimiento</t>
   </si>
@@ -129,6 +129,9 @@
   <si>
     <t>25T1</t>
   </si>
+  <si>
+    <t>25T2</t>
+  </si>
 </sst>
 </file>
 
@@ -137,10 +140,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -765,6 +774,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -772,7 +782,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1262,6 +1271,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1269,7 +1279,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2764,16 +2773,16 @@
   <dimension ref="C1:S50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31:G32"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I1" s="2"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -2786,11 +2795,11 @@
       <c r="R1" s="3"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I2" s="5"/>
       <c r="S2" s="6"/>
     </row>
-    <row r="3" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:19" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
         <v>0</v>
       </c>
@@ -2803,7 +2812,7 @@
       <c r="I3" s="5"/>
       <c r="S3" s="6"/>
     </row>
-    <row r="4" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>2</v>
       </c>
@@ -2817,7 +2826,7 @@
       <c r="I4" s="5"/>
       <c r="S4" s="6"/>
     </row>
-    <row r="5" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>3</v>
       </c>
@@ -2831,7 +2840,7 @@
       <c r="I5" s="5"/>
       <c r="S5" s="6"/>
     </row>
-    <row r="6" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>4</v>
       </c>
@@ -2845,7 +2854,7 @@
       <c r="I6" s="5"/>
       <c r="S6" s="6"/>
     </row>
-    <row r="7" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>5</v>
       </c>
@@ -2863,7 +2872,7 @@
       <c r="I7" s="5"/>
       <c r="S7" s="6"/>
     </row>
-    <row r="8" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>6</v>
       </c>
@@ -2881,7 +2890,7 @@
       <c r="I8" s="5"/>
       <c r="S8" s="6"/>
     </row>
-    <row r="9" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>7</v>
       </c>
@@ -2899,7 +2908,7 @@
       <c r="I9" s="5"/>
       <c r="S9" s="6"/>
     </row>
-    <row r="10" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>8</v>
       </c>
@@ -2917,7 +2926,7 @@
       <c r="I10" s="5"/>
       <c r="S10" s="6"/>
     </row>
-    <row r="11" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>9</v>
       </c>
@@ -2935,7 +2944,7 @@
       <c r="I11" s="5"/>
       <c r="S11" s="6"/>
     </row>
-    <row r="12" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>10</v>
       </c>
@@ -2953,7 +2962,7 @@
       <c r="I12" s="5"/>
       <c r="S12" s="6"/>
     </row>
-    <row r="13" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>11</v>
       </c>
@@ -2971,7 +2980,7 @@
       <c r="I13" s="5"/>
       <c r="S13" s="6"/>
     </row>
-    <row r="14" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>12</v>
       </c>
@@ -2989,7 +2998,7 @@
       <c r="I14" s="5"/>
       <c r="S14" s="6"/>
     </row>
-    <row r="15" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>13</v>
       </c>
@@ -3007,7 +3016,7 @@
       <c r="I15" s="5"/>
       <c r="S15" s="6"/>
     </row>
-    <row r="16" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>14</v>
       </c>
@@ -3025,7 +3034,7 @@
       <c r="I16" s="5"/>
       <c r="S16" s="6"/>
     </row>
-    <row r="17" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>15</v>
       </c>
@@ -3043,7 +3052,7 @@
       <c r="I17" s="5"/>
       <c r="S17" s="6"/>
     </row>
-    <row r="18" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>16</v>
       </c>
@@ -3061,7 +3070,7 @@
       <c r="I18" s="5"/>
       <c r="S18" s="6"/>
     </row>
-    <row r="19" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>17</v>
       </c>
@@ -3079,7 +3088,7 @@
       <c r="I19" s="5"/>
       <c r="S19" s="6"/>
     </row>
-    <row r="20" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>18</v>
       </c>
@@ -3097,7 +3106,7 @@
       <c r="I20" s="5"/>
       <c r="S20" s="6"/>
     </row>
-    <row r="21" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>19</v>
       </c>
@@ -3115,7 +3124,7 @@
       <c r="I21" s="5"/>
       <c r="S21" s="6"/>
     </row>
-    <row r="22" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>20</v>
       </c>
@@ -3133,7 +3142,7 @@
       <c r="I22" s="5"/>
       <c r="S22" s="6"/>
     </row>
-    <row r="23" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>21</v>
       </c>
@@ -3151,7 +3160,7 @@
       <c r="I23" s="5"/>
       <c r="S23" s="6"/>
     </row>
-    <row r="24" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>22</v>
       </c>
@@ -3169,7 +3178,7 @@
       <c r="I24" s="5"/>
       <c r="S24" s="6"/>
     </row>
-    <row r="25" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>23</v>
       </c>
@@ -3187,7 +3196,7 @@
       <c r="I25" s="5"/>
       <c r="S25" s="6"/>
     </row>
-    <row r="26" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>24</v>
       </c>
@@ -3205,7 +3214,7 @@
       <c r="I26" s="5"/>
       <c r="S26" s="6"/>
     </row>
-    <row r="27" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>25</v>
       </c>
@@ -3223,7 +3232,7 @@
       <c r="I27" s="5"/>
       <c r="S27" s="6"/>
     </row>
-    <row r="28" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>26</v>
       </c>
@@ -3241,7 +3250,7 @@
       <c r="I28" s="5"/>
       <c r="S28" s="6"/>
     </row>
-    <row r="29" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>27</v>
       </c>
@@ -3259,7 +3268,7 @@
       <c r="I29" s="5"/>
       <c r="S29" s="6"/>
     </row>
-    <row r="30" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>28</v>
       </c>
@@ -3277,7 +3286,7 @@
       <c r="I30" s="5"/>
       <c r="S30" s="6"/>
     </row>
-    <row r="31" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>29</v>
       </c>
@@ -3295,7 +3304,7 @@
       <c r="I31" s="5"/>
       <c r="S31" s="6"/>
     </row>
-    <row r="32" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>30</v>
       </c>
@@ -3313,50 +3322,62 @@
       <c r="I32" s="5"/>
       <c r="S32" s="6"/>
     </row>
-    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="E33" s="1"/>
-      <c r="G33" s="1"/>
+    <row r="33" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="F33">
+        <f t="shared" ref="F33" si="6">F32*(1+E33/100)</f>
+        <v>112.70801467572858</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" ref="G33" si="7">((F33/F29)-1)*100</f>
+        <v>3.0333604834999583</v>
+      </c>
       <c r="I33" s="5"/>
       <c r="S33" s="6"/>
     </row>
-    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:19" x14ac:dyDescent="0.3">
       <c r="E34" s="1"/>
       <c r="G34" s="1"/>
       <c r="I34" s="5"/>
       <c r="S34" s="6"/>
     </row>
-    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:19" x14ac:dyDescent="0.3">
       <c r="E35" s="1"/>
       <c r="G35" s="1"/>
       <c r="I35" s="5"/>
       <c r="S35" s="6"/>
     </row>
-    <row r="36" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:19" x14ac:dyDescent="0.3">
       <c r="E36" s="1"/>
       <c r="G36" s="1"/>
       <c r="I36" s="5"/>
       <c r="S36" s="6"/>
     </row>
-    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:19" x14ac:dyDescent="0.3">
       <c r="E37" s="1"/>
       <c r="G37" s="1"/>
       <c r="I37" s="5"/>
       <c r="S37" s="6"/>
     </row>
-    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:19" x14ac:dyDescent="0.3">
       <c r="E38" s="1"/>
       <c r="G38" s="1"/>
       <c r="I38" s="5"/>
       <c r="S38" s="6"/>
     </row>
-    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:19" x14ac:dyDescent="0.3">
       <c r="D39">
         <v>100</v>
       </c>
       <c r="I39" s="5"/>
       <c r="S39" s="6"/>
     </row>
-    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C40" s="1">
         <f>E21</f>
         <v>1.7</v>
@@ -3368,13 +3389,13 @@
       <c r="I40" s="5"/>
       <c r="S40" s="6"/>
     </row>
-    <row r="41" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
-        <f t="shared" ref="C41:C50" si="6">E22</f>
+        <f t="shared" ref="C41:C50" si="8">E22</f>
         <v>0.5</v>
       </c>
       <c r="D41">
-        <f t="shared" ref="D41:D48" si="7">D40*(1+C41/100)</f>
+        <f t="shared" ref="D41:D48" si="9">D40*(1+C41/100)</f>
         <v>102.20849999999997</v>
       </c>
       <c r="I41" s="7"/>
@@ -3389,13 +3410,13 @@
       <c r="R41" s="8"/>
       <c r="S41" s="9"/>
     </row>
-    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C42" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.5</v>
       </c>
       <c r="D42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>102.71954249999996</v>
       </c>
       <c r="E42">
@@ -3403,43 +3424,43 @@
         <v>101.65701062499997</v>
       </c>
     </row>
-    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C43" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.7</v>
       </c>
       <c r="D43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>103.43857929749996</v>
       </c>
     </row>
-    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C44" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.3</v>
       </c>
       <c r="D44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>103.74889503539245</v>
       </c>
     </row>
-    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C45" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
       <c r="D45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>103.95639282546324</v>
       </c>
     </row>
-    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C46" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.8</v>
       </c>
       <c r="D46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>104.78804396806694</v>
       </c>
       <c r="E46">
@@ -3451,29 +3472,29 @@
         <v>2.2880538610228207</v>
       </c>
     </row>
-    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C47" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>105.83592440774761</v>
       </c>
     </row>
-    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C48" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.9</v>
       </c>
       <c r="D48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>106.78844772741733</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C49" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.9</v>
       </c>
       <c r="D49">
@@ -3481,9 +3502,9 @@
         <v>107.74954375696409</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C50" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.9</v>
       </c>
       <c r="D50">
@@ -3500,6 +3521,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>